<commit_message>
Update MID - Campos obligatorios entidades.xlsx
Campos oblig
</commit_message>
<xml_diff>
--- a/6- Ingenieria de producto/6.1 - Análisis/04- Archivos de Trabajo/MID - Campos obligatorios entidades.xlsx
+++ b/6- Ingenieria de producto/6.1 - Análisis/04- Archivos de Trabajo/MID - Campos obligatorios entidades.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="24" windowWidth="7140" windowHeight="8496"/>
+    <workbookView xWindow="288" yWindow="24" windowWidth="7140" windowHeight="8496" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Obligatorios" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Datos Obligatorios 1" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
   <si>
     <t>Caja</t>
   </si>
@@ -127,6 +128,12 @@
   </si>
   <si>
     <t xml:space="preserve">Registrar alta de Entidades / Designar Datos Obligatorios </t>
+  </si>
+  <si>
+    <t>Gobierno</t>
+  </si>
+  <si>
+    <t>Justicia</t>
   </si>
 </sst>
 </file>
@@ -416,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -452,6 +459,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -467,12 +480,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -481,6 +488,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,33 +829,33 @@
       <c r="I2" s="26"/>
     </row>
     <row r="3" spans="2:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -1066,11 +1079,11 @@
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1176,11 +1189,11 @@
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
@@ -1272,11 +1285,11 @@
       <c r="I34" s="12"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
@@ -1368,11 +1381,11 @@
       <c r="I41" s="12"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="19"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
@@ -1452,13 +1465,667 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="2.77734375" customWidth="1"/>
+    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="0.77734375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="2:10" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="27"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="2">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="2">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="2">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="2">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="2">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="2">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+      <c r="C18" s="2">
+        <v>14</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+      <c r="C19" s="10">
+        <v>15</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="2">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+      <c r="C26" s="10">
+        <v>6</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="3"/>
+      <c r="C27" s="10">
+        <v>7</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="3"/>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="3"/>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+      <c r="C32" s="2">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="3"/>
+      <c r="C33" s="10">
+        <v>5</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="3"/>
+      <c r="C34" s="10">
+        <v>6</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="3"/>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="3"/>
+      <c r="C37" s="2">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="3"/>
+      <c r="C38" s="2">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="3"/>
+      <c r="C39" s="2">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="3"/>
+      <c r="C40" s="10">
+        <v>5</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="3"/>
+      <c r="C41" s="10">
+        <v>6</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="3"/>
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="3"/>
+      <c r="C44" s="2">
+        <v>2</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B45" s="3"/>
+      <c r="C45" s="2">
+        <v>3</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+    </row>
+    <row r="46" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="4"/>
+      <c r="C46" s="5">
+        <v>4</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B35:D35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1472,4 +2139,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>